<commit_message>
Workin on the Pie Chart
</commit_message>
<xml_diff>
--- a/Lyric Analysis/Resources/Excel Files/Pop.xlsx
+++ b/Lyric Analysis/Resources/Excel Files/Pop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="366">
   <si>
     <t>You</t>
   </si>
@@ -59,9 +59,6 @@
     <t>To</t>
   </si>
   <si>
-    <t>The</t>
-  </si>
-  <si>
     <t>Huh</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Regret</t>
   </si>
   <si>
-    <t>And</t>
-  </si>
-  <si>
     <t>Expect</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
   </si>
   <si>
     <t>Believer</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>Pain</t>
@@ -1456,7 +1447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1579,7 +1570,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1611,7 +1602,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1675,7 +1666,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1699,7 +1690,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1827,7 +1818,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1979,7 +1970,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1987,7 +1978,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2027,7 +2018,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2035,7 +2026,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2163,22 +2154,6 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>88</v>
-      </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>89</v>
-      </c>
-      <c r="B90">
         <v>1</v>
       </c>
     </row>
@@ -2189,7 +2164,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B130"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2197,111 +2172,111 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B1">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -2309,79 +2284,79 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19">
         <v>4</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2389,7 +2364,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -2472,28 +2447,28 @@
         <v>110</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -2501,7 +2476,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -2509,7 +2484,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -2517,7 +2492,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -2525,7 +2500,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -2533,7 +2508,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -2541,7 +2516,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -2589,7 +2564,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -2597,7 +2572,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>43</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -2605,7 +2580,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -2613,7 +2588,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -2621,7 +2596,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -2704,7 +2679,7 @@
         <v>134</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2712,7 +2687,7 @@
         <v>135</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2720,7 +2695,7 @@
         <v>136</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2757,7 +2732,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2765,7 +2740,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2773,7 +2748,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2781,7 +2756,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2789,7 +2764,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2797,7 +2772,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2805,7 +2780,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2813,7 +2788,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2821,7 +2796,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2829,7 +2804,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -3021,7 +2996,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>61</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -3029,7 +3004,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -3037,7 +3012,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -3045,7 +3020,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>63</v>
+        <v>171</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -3053,7 +3028,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -3189,7 +3164,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>189</v>
+        <v>16</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -3197,7 +3172,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -3205,33 +3180,9 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" t="s">
-        <v>17</v>
-      </c>
-      <c r="B128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" t="s">
-        <v>70</v>
-      </c>
-      <c r="B129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" t="s">
-        <v>192</v>
-      </c>
-      <c r="B130">
         <v>1</v>
       </c>
     </row>
@@ -3242,7 +3193,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3266,15 +3217,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -3282,15 +3233,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -3298,7 +3249,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -3306,55 +3257,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -3362,23 +3313,23 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -3386,7 +3337,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -3394,7 +3345,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>81</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -3402,7 +3353,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -3410,7 +3361,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>198</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -3418,7 +3369,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -3426,7 +3377,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -3434,7 +3385,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -3442,7 +3393,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="B25">
         <v>6</v>
@@ -3450,7 +3401,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>201</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -3458,39 +3409,39 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>205</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -3498,7 +3449,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -3506,7 +3457,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -3514,7 +3465,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>205</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -3522,7 +3473,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -3530,10 +3481,10 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3541,7 +3492,7 @@
         <v>208</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3549,12 +3500,12 @@
         <v>209</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>210</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -3562,7 +3513,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>154</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -3570,7 +3521,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3578,7 +3529,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -3586,7 +3537,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>54</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -3594,7 +3545,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -3602,7 +3553,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>212</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -3610,7 +3561,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>213</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -3634,7 +3585,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -3642,7 +3593,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>20</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -3650,7 +3601,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>111</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -3658,7 +3609,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -3666,7 +3617,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -3674,7 +3625,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -3682,31 +3633,31 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>217</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -3714,7 +3665,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>219</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -3722,7 +3673,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>220</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -3738,7 +3689,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>135</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -3746,7 +3697,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>223</v>
+        <v>16</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -3754,7 +3705,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>49</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -3762,7 +3713,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -3770,7 +3721,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>223</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -3778,7 +3729,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>50</v>
+        <v>224</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -3818,7 +3769,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>229</v>
+        <v>21</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -3826,7 +3777,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>230</v>
+        <v>108</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -3834,7 +3785,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -3842,7 +3793,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -3850,7 +3801,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>231</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -3946,7 +3897,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>243</v>
+        <v>24</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -3954,7 +3905,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -3962,7 +3913,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -3970,7 +3921,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>25</v>
+        <v>245</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -4018,7 +3969,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>251</v>
+        <v>138</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -4026,7 +3977,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -4034,7 +3985,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -4042,7 +3993,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>141</v>
+        <v>252</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -4050,7 +4001,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -4058,7 +4009,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -4066,7 +4017,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>255</v>
+        <v>122</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -4074,7 +4025,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>256</v>
+        <v>66</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -4082,7 +4033,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>86</v>
+        <v>254</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -4090,7 +4041,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -4098,7 +4049,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>68</v>
+        <v>255</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -4106,7 +4057,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -4114,7 +4065,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>126</v>
+        <v>257</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -4170,7 +4121,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>264</v>
+        <v>6</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -4178,7 +4129,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -4186,33 +4137,9 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" t="s">
-        <v>6</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
-        <v>267</v>
-      </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" t="s">
-        <v>268</v>
-      </c>
-      <c r="B121">
         <v>1</v>
       </c>
     </row>
@@ -4223,7 +4150,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4231,7 +4158,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B1">
         <v>20</v>
@@ -4255,7 +4182,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -4271,7 +4198,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -4279,7 +4206,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -4287,7 +4214,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -4295,31 +4222,31 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>220</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>269</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>270</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -4327,23 +4254,23 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>273</v>
+        <v>24</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -4351,7 +4278,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -4359,7 +4286,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>272</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -4367,23 +4294,23 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>274</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -4391,7 +4318,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -4399,7 +4326,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -4407,7 +4334,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -4415,7 +4342,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -4423,7 +4350,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>279</v>
+        <v>0</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -4431,7 +4358,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -4439,7 +4366,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>279</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -4447,7 +4374,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>281</v>
+        <v>152</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -4455,7 +4382,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -4463,7 +4390,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>281</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -4471,7 +4398,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -4479,7 +4406,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -4487,7 +4414,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>285</v>
+        <v>238</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -4495,7 +4422,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>286</v>
+        <v>12</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -4503,23 +4430,23 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>241</v>
+        <v>284</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -4527,7 +4454,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>286</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -4535,7 +4462,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -4543,7 +4470,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -4551,7 +4478,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -4559,7 +4486,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>291</v>
+        <v>4</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -4567,7 +4494,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>292</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -4575,7 +4502,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>290</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -4583,7 +4510,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>291</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -4591,7 +4518,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -4599,23 +4526,23 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4623,7 +4550,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4631,7 +4558,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4639,7 +4566,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4647,7 +4574,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4655,7 +4582,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -4663,7 +4590,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>302</v>
+        <v>58</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -4671,7 +4598,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>303</v>
+        <v>192</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -4679,7 +4606,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>301</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -4687,7 +4614,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>195</v>
+        <v>302</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -4695,7 +4622,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -4703,7 +4630,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4711,7 +4638,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>306</v>
+        <v>109</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -4719,7 +4646,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -4727,7 +4654,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>112</v>
+        <v>306</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -4735,7 +4662,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>308</v>
+        <v>235</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4743,7 +4670,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4751,7 +4678,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>238</v>
+        <v>308</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4759,7 +4686,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4767,7 +4694,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -4775,7 +4702,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -4783,7 +4710,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>312</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -4815,7 +4742,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>316</v>
+        <v>95</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -4823,7 +4750,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -4831,33 +4758,9 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>98</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
-        <v>319</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>320</v>
-      </c>
-      <c r="B79">
         <v>1</v>
       </c>
     </row>
@@ -4868,7 +4771,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4876,7 +4779,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1">
         <v>34</v>
@@ -4884,7 +4787,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>25</v>
@@ -4892,7 +4795,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B3">
         <v>24</v>
@@ -4916,15 +4819,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -4932,7 +4835,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -4940,7 +4843,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>232</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -4948,159 +4851,159 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>319</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>322</v>
+        <v>108</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>320</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>236</v>
+        <v>27</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>267</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>323</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>270</v>
+        <v>112</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>321</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>242</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>324</v>
+        <v>53</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>245</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>322</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>323</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>324</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>325</v>
+        <v>276</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -5108,7 +5011,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>326</v>
+        <v>192</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -5116,7 +5019,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -5124,7 +5027,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>279</v>
+        <v>326</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -5132,7 +5035,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -5140,7 +5043,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>328</v>
+        <v>47</v>
       </c>
       <c r="B34">
         <v>4</v>
@@ -5148,7 +5051,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>329</v>
+        <v>193</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -5156,26 +5059,26 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>327</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>328</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>329</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5196,7 +5099,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>332</v>
+        <v>32</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -5204,7 +5107,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -5212,7 +5115,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -5220,7 +5123,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -5228,7 +5131,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>335</v>
+        <v>7</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -5236,7 +5139,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>336</v>
+        <v>183</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -5244,7 +5147,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -5252,7 +5155,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>334</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -5260,7 +5163,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>186</v>
+        <v>335</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -5268,7 +5171,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -5276,7 +5179,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>337</v>
+        <v>187</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -5284,7 +5187,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -5292,31 +5195,31 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>339</v>
+        <v>279</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>198</v>
+        <v>337</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -5324,7 +5227,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5332,7 +5235,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5340,7 +5243,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>340</v>
+        <v>191</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -5348,7 +5251,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>339</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -5356,7 +5259,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>341</v>
+        <v>77</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -5364,7 +5267,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>194</v>
+        <v>340</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -5372,7 +5275,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>342</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -5380,7 +5283,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -5388,7 +5291,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -5396,7 +5299,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -5404,7 +5307,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -5412,7 +5315,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>344</v>
+        <v>141</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -5420,7 +5323,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>343</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -5428,7 +5331,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>345</v>
+        <v>270</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -5436,31 +5339,31 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>344</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>273</v>
+        <v>346</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>347</v>
+        <v>123</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -5468,7 +5371,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>348</v>
+        <v>46</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -5476,7 +5379,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>349</v>
+        <v>16</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -5484,7 +5387,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -5492,7 +5395,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>347</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -5500,7 +5403,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>201</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -5508,7 +5411,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>52</v>
+        <v>348</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -5516,7 +5419,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -5524,7 +5427,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -5532,7 +5435,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -5540,7 +5443,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -5548,7 +5451,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -5556,7 +5459,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -5564,7 +5467,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -5572,7 +5475,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5580,7 +5483,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -5588,7 +5491,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -5596,7 +5499,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>114</v>
+        <v>235</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -5604,7 +5507,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -5612,7 +5515,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -5620,7 +5523,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>238</v>
+        <v>358</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -5628,7 +5531,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>359</v>
+        <v>62</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -5636,7 +5539,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -5644,7 +5547,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -5652,7 +5555,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -5660,7 +5563,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>362</v>
+        <v>81</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -5668,7 +5571,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -5676,7 +5579,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>362</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -5684,7 +5587,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>83</v>
+        <v>363</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -5692,7 +5595,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>364</v>
+        <v>227</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -5700,7 +5603,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -5708,7 +5611,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>366</v>
+        <v>248</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -5716,7 +5619,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>230</v>
+        <v>365</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -5724,33 +5627,9 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>367</v>
+        <v>9</v>
       </c>
       <c r="B107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
-        <v>251</v>
-      </c>
-      <c r="B108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
-        <v>368</v>
-      </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110">
         <v>1</v>
       </c>
     </row>

</xml_diff>